<commit_message>
Added NP root and tip alignments for EVEs
</commit_message>
<xml_diff>
--- a/tabular/eve-side-data.xlsx
+++ b/tabular/eve-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32820" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1556,8 +1556,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1595,7 +1623,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1609,6 +1637,20 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1622,6 +1664,20 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1953,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="L111" sqref="L111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>